<commit_message>
Version 2.0 For QA Processes
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="3495" windowWidth="19425" windowHeight="10425"/>
+    <workbookView xWindow="-105" yWindow="4395" windowWidth="19425" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="59">
   <si>
     <t>Name</t>
   </si>
@@ -184,6 +184,24 @@
   </si>
   <si>
     <t>Buen día, ocurrió un error en el bot de Salvamentos, se adjunta ScreenShot. Saludos.</t>
+  </si>
+  <si>
+    <t>FolderLayout</t>
+  </si>
+  <si>
+    <t>Data/Input/</t>
+  </si>
+  <si>
+    <t>UserAccountError</t>
+  </si>
+  <si>
+    <t>Es la cuenta de Outlook configurada en la computadora</t>
+  </si>
+  <si>
+    <t>SearchCriteria</t>
+  </si>
+  <si>
+    <t>Lote de Facturas y PDF a descargar</t>
   </si>
 </sst>
 </file>
@@ -570,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -698,6 +716,9 @@
       <c r="B15" s="5" t="s">
         <v>42</v>
       </c>
+      <c r="C15" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
@@ -742,7 +763,7 @@
     </row>
     <row r="22" spans="1:2" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>42</v>
@@ -757,8 +778,22 @@
       </c>
     </row>
     <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26" t="s">
+        <v>58</v>
+      </c>
+    </row>
     <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:2" ht="14.25" customHeight="1"/>

</xml_diff>